<commit_message>
Adicionada REC de ALP
</commit_message>
<xml_diff>
--- a/CST_ATP_2025.xlsx
+++ b/CST_ATP_2025.xlsx
@@ -356,7 +356,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -395,10 +395,10 @@
       <c r="J1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>202510705410</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="2"/>
@@ -407,10 +407,10 @@
       <c r="I2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>202510705418</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2"/>
@@ -423,10 +423,10 @@
       <c r="J3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>202510706076</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="2"/>
@@ -435,10 +435,10 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>202510706080</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="2" t="n">
@@ -455,10 +455,10 @@
       <c r="J5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>202510704356</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="2"/>
@@ -471,10 +471,10 @@
       <c r="J6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>202510704359</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="2" t="n">
@@ -491,10 +491,10 @@
       <c r="J7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>202510704126</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="2" t="n">
@@ -510,10 +510,10 @@
       <c r="I8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>202510706847</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="2"/>
@@ -526,10 +526,10 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>202510704129</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="2" t="n">
@@ -548,10 +548,10 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>202510704365</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="2" t="n">
@@ -568,10 +568,10 @@
       <c r="J11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>202510706125</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="2" t="n">
@@ -583,17 +583,19 @@
       <c r="E12" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2" t="n">
+        <v>10</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>202510706135</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="2"/>
@@ -602,10 +604,10 @@
       <c r="I13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>202510706851</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="2" t="n">
@@ -624,27 +626,30 @@
       <c r="J14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>202510704132</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="F15" s="1" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>202510704367</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="2" t="n">
@@ -657,10 +662,10 @@
       <c r="I16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>202510704139</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="2" t="n">
@@ -672,244 +677,267 @@
       <c r="E17" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2" t="n">
+        <v>8</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="1" t="n">
         <v>202510706148</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <v>202510704146</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="F19" s="1" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <v>202510704369</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="F20" s="1" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>202510705420</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+      <c r="A22" s="1" t="n">
         <v>202510705417</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="E22" s="0" t="n">
+      <c r="C22" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E22" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+      <c r="A23" s="1" t="n">
         <v>202510706157</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C23" s="1" t="n">
         <v>6</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="F23" s="1" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+      <c r="A24" s="1" t="n">
         <v>202510704351</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="C24" s="1" t="n">
         <v>6</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E24" s="0" t="n">
-        <v>6</v>
+      <c r="E24" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+      <c r="A25" s="1" t="n">
         <v>202510704374</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="E25" s="0" t="n">
+      <c r="C25" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="E25" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="F25" s="1" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+      <c r="A26" s="1" t="n">
         <v>202510704352</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="E26" s="0" t="n">
+      <c r="C26" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E26" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="A27" s="1" t="n">
         <v>202510706162</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
+      <c r="A28" s="1" t="n">
         <v>202510706165</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C28" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="E28" s="0" t="n">
-        <v>4</v>
+      <c r="E28" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+      <c r="A29" s="1" t="n">
         <v>202510708629</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+      <c r="A30" s="1" t="n">
         <v>202510704353</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="C30" s="1" t="n">
         <v>6</v>
       </c>
       <c r="D30" s="1" t="n">
         <v>8</v>
       </c>
+      <c r="F30" s="1" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+      <c r="A31" s="1" t="n">
         <v>202310203444</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
+      <c r="A32" s="1" t="n">
         <v>202510704376</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="E32" s="0" t="n">
+      <c r="C32" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E32" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
+      <c r="A33" s="1" t="n">
         <v>202510704380</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="E33" s="0" t="n">
+      <c r="C33" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="E33" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
+      <c r="A34" s="1" t="n">
         <v>202510704354</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D34" s="1" t="n">
@@ -917,34 +945,40 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
+      <c r="A35" s="1" t="n">
         <v>202510706174</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="E35" s="0" t="n">
+      <c r="C35" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="E35" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="F35" s="1" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
+      <c r="A36" s="1" t="n">
         <v>202510704355</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="0" t="n">
+      <c r="C36" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D36" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="E36" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="F36" s="1" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>